<commit_message>
Updated Information based on Session 3
</commit_message>
<xml_diff>
--- a/Minaria Cheatsheet.xlsx
+++ b/Minaria Cheatsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>NPC Names</t>
   </si>
@@ -43,6 +43,12 @@
     <t>Tiefling</t>
   </si>
   <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Allignments</t>
+  </si>
+  <si>
     <t>Boreaeg Hillfeet</t>
   </si>
   <si>
@@ -400,7 +406,7 @@
     <t>Zestari Holabella</t>
   </si>
   <si>
-    <t>Marble</t>
+    <t>Jade</t>
   </si>
   <si>
     <t>Oih</t>
@@ -562,7 +568,7 @@
     <t>Virion Erkas</t>
   </si>
   <si>
-    <t>Whistle</t>
+    <t>Tumult</t>
   </si>
   <si>
     <t>Pug</t>
@@ -675,10 +681,10 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1023,517 +1029,523 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>1.0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2.0</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>3.0</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>4.0</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>5.0</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>6.0</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>56</v>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="I8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>7.0</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>65</v>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>8.0</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>74</v>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8">
         <v>9.0</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>83</v>
+      <c r="B11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8">
         <v>10.0</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>92</v>
+      <c r="B12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>99</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8">
         <v>11.0</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>101</v>
+      <c r="B13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8">
         <v>12.0</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>110</v>
+      <c r="B14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>117</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8">
         <v>13.0</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>119</v>
+      <c r="B15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>126</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8">
         <v>14.0</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>128</v>
+      <c r="B16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>135</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8">
         <v>15.0</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>137</v>
+      <c r="B17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>144</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8">
         <v>16.0</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>146</v>
+      <c r="B18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F18" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="H18" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J18" s="3" t="s">
         <v>153</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="19">
@@ -1541,31 +1553,31 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20">
@@ -1573,31 +1585,31 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21">
@@ -1605,31 +1617,31 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
@@ -1637,31 +1649,31 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
End of Year Wifcaster Update
</commit_message>
<xml_diff>
--- a/Minaria Cheatsheet.xlsx
+++ b/Minaria Cheatsheet.xlsx
@@ -55,7 +55,7 @@
     <t>Folwin Liahice</t>
   </si>
   <si>
-    <t>River</t>
+    <t>Splash</t>
   </si>
   <si>
     <t>Asb</t>
@@ -82,7 +82,7 @@
     <t>Vulas Farran</t>
   </si>
   <si>
-    <t>Basin</t>
+    <t>Brine</t>
   </si>
   <si>
     <t>Bliord</t>
@@ -133,7 +133,7 @@
     <t>Lorhom Bronzehelm</t>
   </si>
   <si>
-    <t>Ralnor Beifiel</t>
+    <t>Cyran Herqen</t>
   </si>
   <si>
     <t>Arson</t>
@@ -190,7 +190,7 @@
     <t>Darcassan Kelrie</t>
   </si>
   <si>
-    <t>Slab</t>
+    <t>Quartz</t>
   </si>
   <si>
     <t>Blic</t>
@@ -352,7 +352,7 @@
     <t>Lusha Faxisys</t>
   </si>
   <si>
-    <t>Cinder</t>
+    <t>Kindle</t>
   </si>
   <si>
     <t>Pas</t>
@@ -460,7 +460,7 @@
     <t>Vestele Faero</t>
   </si>
   <si>
-    <t>Drift</t>
+    <t>Flurry</t>
   </si>
   <si>
     <t>Reesh</t>
@@ -674,14 +674,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -691,6 +691,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -998,41 +1001,70 @@
     <col customWidth="1" min="9" max="9" width="21.25"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1040,31 +1072,31 @@
       <c r="A3" s="3">
         <v>1.0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1072,31 +1104,31 @@
       <c r="A4" s="3">
         <v>2.0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1104,31 +1136,31 @@
       <c r="A5" s="3">
         <v>3.0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1136,31 +1168,31 @@
       <c r="A6" s="3">
         <v>4.0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1168,31 +1200,31 @@
       <c r="A7" s="3">
         <v>5.0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1200,31 +1232,31 @@
       <c r="A8" s="3">
         <v>6.0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1232,31 +1264,31 @@
       <c r="A9" s="3">
         <v>7.0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1264,429 +1296,429 @@
       <c r="A10" s="3">
         <v>8.0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>9.0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>10.0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>11.0</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>12.0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>13.0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>14.0</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8">
+      <c r="A17" s="9">
         <v>15.0</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="8">
+      <c r="A18" s="9">
         <v>16.0</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10">
+      <c r="A19" s="11">
         <v>17.0</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="10" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>18.0</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>166</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="10" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10">
+      <c r="A21" s="11">
         <v>19.0</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="10" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10">
+      <c r="A22" s="11">
         <v>20.0</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="10" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="23">
-      <c r="D23" s="11"/>
+      <c r="D23" s="12"/>
     </row>
     <row r="24">
-      <c r="D24" s="11"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25">
-      <c r="D25" s="11"/>
+      <c r="D25" s="12"/>
     </row>
     <row r="26">
-      <c r="D26" s="11"/>
+      <c r="D26" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>